<commit_message>
Network Wall Port document updates for EShop
</commit_message>
<xml_diff>
--- a/HCRO-Network-Infrastructure/Mainlab Network Wall Ports.xlsx
+++ b/HCRO-Network-Infrastructure/Mainlab Network Wall Ports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smeyers/Documents/GitHubSETI/Front-Page/HCRO-Network-Infrastructure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C80173-CB47-7941-8BAA-078A4F9CEA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3D1422-0CED-EE4D-80A5-3657871504D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16460" yWindow="8420" windowWidth="27640" windowHeight="16940" xr2:uid="{4E213348-FF62-B440-B59C-815E7F096F2E}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$71</definedName>
   </definedNames>
   <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="37">
   <si>
     <t>Room</t>
   </si>
@@ -134,13 +134,22 @@
     <t>Electronics Shop</t>
   </si>
   <si>
-    <t>West Wall on Bench Left Side</t>
-  </si>
-  <si>
-    <t>West Wall on Bench Right Side</t>
-  </si>
-  <si>
-    <t>North Wall Low Next to Double Door</t>
+    <t>South-West Wall on Bench Left Side</t>
+  </si>
+  <si>
+    <t>South-West Wall on Bench Right Side</t>
+  </si>
+  <si>
+    <t>North-East Wall Low Next to Double Door</t>
+  </si>
+  <si>
+    <t>Signal Processing Room</t>
+  </si>
+  <si>
+    <t>Security Panel</t>
+  </si>
+  <si>
+    <t>Fire Panel</t>
   </si>
 </sst>
 </file>
@@ -520,16 +529,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB022DAA-1B20-E745-BC0A-55D8341CF941}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -551,13 +560,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -565,13 +574,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -579,13 +588,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -593,13 +602,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -607,13 +616,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -621,13 +630,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
         <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -635,13 +644,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
         <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -649,13 +658,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -663,13 +672,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,13 +686,13 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -691,13 +700,13 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -705,41 +714,41 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
       </c>
       <c r="D14">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -772,35 +781,35 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
         <v>11</v>
       </c>
       <c r="D19">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
@@ -809,12 +818,12 @@
         <v>5</v>
       </c>
       <c r="D20">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
@@ -823,91 +832,91 @@
         <v>5</v>
       </c>
       <c r="D21">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
       <c r="D27">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -968,142 +977,142 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
       </c>
       <c r="D34">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
       </c>
       <c r="D35">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
         <v>21</v>
       </c>
       <c r="D36">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
         <v>21</v>
       </c>
       <c r="D37">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
         <v>21</v>
       </c>
       <c r="D38">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
         <v>21</v>
       </c>
       <c r="D39">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
         <v>21</v>
       </c>
       <c r="D40">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C41" t="s">
         <v>21</v>
       </c>
       <c r="D41">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1111,13 +1120,13 @@
         <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
       </c>
       <c r="D42">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1125,13 +1134,13 @@
         <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1195,13 +1204,13 @@
         <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C48" t="s">
         <v>21</v>
       </c>
       <c r="D48">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1209,13 +1218,13 @@
         <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C49" t="s">
         <v>21</v>
       </c>
       <c r="D49">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1243,7 +1252,7 @@
         <v>21</v>
       </c>
       <c r="D51">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1251,13 +1260,13 @@
         <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C52" t="s">
         <v>21</v>
       </c>
       <c r="D52">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1265,13 +1274,13 @@
         <v>23</v>
       </c>
       <c r="B53" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C53" t="s">
         <v>21</v>
       </c>
       <c r="D53">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1313,7 +1322,7 @@
         <v>21</v>
       </c>
       <c r="D56">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1327,135 +1336,147 @@
         <v>21</v>
       </c>
       <c r="D57">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B58" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C58" t="s">
         <v>21</v>
       </c>
       <c r="D58">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C59" t="s">
         <v>21</v>
       </c>
       <c r="D59">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C60" t="s">
         <v>11</v>
       </c>
       <c r="D60">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B61" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C61" t="s">
         <v>11</v>
       </c>
       <c r="D61">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B62" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C62" t="s">
         <v>21</v>
       </c>
       <c r="D62">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C63" t="s">
         <v>21</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C64" t="s">
         <v>21</v>
       </c>
       <c r="D64">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C65" t="s">
         <v>21</v>
       </c>
       <c r="D65">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="C66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66">
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>31</v>
+        <v>20</v>
+      </c>
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67">
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1465,6 +1486,12 @@
       <c r="B68" t="s">
         <v>32</v>
       </c>
+      <c r="C68" t="s">
+        <v>21</v>
+      </c>
+      <c r="D68">
+        <v>23</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -1473,25 +1500,78 @@
       <c r="B69" t="s">
         <v>32</v>
       </c>
+      <c r="C69" t="s">
+        <v>21</v>
+      </c>
+      <c r="D69">
+        <v>24</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>33</v>
+        <v>10</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70">
+        <v>21</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>33</v>
+        <v>10</v>
+      </c>
+      <c r="C71" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" t="s">
+        <v>35</v>
+      </c>
+      <c r="C72" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" t="s">
+        <v>36</v>
+      </c>
+      <c r="C73" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{BB022DAA-1B20-E745-BC0A-55D8341CF941}"/>
+  <autoFilter ref="A1:D71" xr:uid="{BB022DAA-1B20-E745-BC0A-55D8341CF941}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:D71">
+      <sortCondition ref="D1:D71"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D72">
+    <sortCondition ref="D1:D72"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>